<commit_message>
:hammer: Add group csv file generator from xlsx file
</commit_message>
<xml_diff>
--- a/candidate-data/datasheets/candidate_data_final.xlsx
+++ b/candidate-data/datasheets/candidate_data_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sawzedong/Desktop/Infocomm/Others/sc-election/candidate-data/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248319DD-04A9-EE45-898D-86B370BFF2C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F365CCA-6354-0146-9AFA-651591D1569E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jh_candidate_data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>id</t>
   </si>
@@ -162,9 +162,6 @@
     <t>J04</t>
   </si>
   <si>
-    <t>J05</t>
-  </si>
-  <si>
     <t>DH19</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
   </si>
   <si>
     <t>S04</t>
-  </si>
-  <si>
-    <t>S05</t>
   </si>
   <si>
     <t>there must be no duplicates of group_id across jh and sh candidates</t>
@@ -664,7 +658,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C65536"/>
+      <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -781,7 +775,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -792,7 +786,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -825,7 +819,7 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -836,7 +830,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +852,7 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,7 +863,7 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,7 +874,7 @@
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -892,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,200 +910,200 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
       </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" t="s">
-        <v>82</v>
-      </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1145,7 +1139,7 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1159,12 +1153,12 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>

</xml_diff>